<commit_message>
change : Show Cam REnewal
</commit_message>
<xml_diff>
--- a/Plugins/ShowActionSystem/Content/SampleData/Excel/TestStructArray.xlsx
+++ b/Plugins/ShowActionSystem/Content/SampleData/Excel/TestStructArray.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unreal Projects\ShowSystemSample\Plugins\ShowActionSystem\Content\SampleData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F75BF19-875D-4188-B7F1-2E8FD742B5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6E756E-CE78-47E1-9483-114D5407FE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33960" yWindow="4140" windowWidth="21600" windowHeight="11835" xr2:uid="{35BD57ED-8C1C-49E5-9B53-6FCBBF09E4FC}"/>
+    <workbookView xWindow="30465" yWindow="195" windowWidth="25800" windowHeight="15345" xr2:uid="{35BD57ED-8C1C-49E5-9B53-6FCBBF09E4FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>RowName</t>
   </si>
@@ -123,6 +123,98 @@
   </si>
   <si>
     <t>TestStrcut3.TestStrcut2.Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>---</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bools</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FormatVer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DataVer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartLine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S:EffectData:Int32</t>
+  </si>
+  <si>
+    <t>S:EffectData:String</t>
+  </si>
+  <si>
+    <t>A(S:EffectData:Int32)</t>
+  </si>
+  <si>
+    <t>A(S:EffectData:String)</t>
+  </si>
+  <si>
+    <t>EffectData.ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectData.Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectDatas.ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectDatas.Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExecSet.EffectData.ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExecSet.EffectData.Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExecSet.EffectDatas.ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExecSet.EffectDatas.Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExecSet.ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S:ExecSet:Int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S:ExecSet:EffectData:Int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S:ExecSet:EffectData:String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S:ExecSet:A(S:EffectData:Int32)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S:ExecSet:A(S:EffectData:String)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -169,9 +261,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,10 +605,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941BA41F-F780-480E-BA57-9B5F8C5A879F}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B18" sqref="B17:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BDEBE7-288F-4A68-B988-1DA33BB35C28}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -627,128 +865,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BDEBE7-288F-4A68-B988-1DA33BB35C28}">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>